<commit_message>
submissions today to compare lbm and catboost /wo upsampling
</commit_message>
<xml_diff>
--- a/data/results/result.xlsx
+++ b/data/results/result.xlsx
@@ -1,37 +1,132 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandro\repo\data_science_for_business_lmu\data\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A919D15-D28F-4C66-9497-AE3568159CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="45" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+  <si>
+    <t>feature_set</t>
+  </si>
+  <si>
+    <t>hp_early_stopping_rounds</t>
+  </si>
+  <si>
+    <t>hp_iterations</t>
+  </si>
+  <si>
+    <t>hp_learning_rate</t>
+  </si>
+  <si>
+    <t>hp_loss_function</t>
+  </si>
+  <si>
+    <t>hp_n_estimators</t>
+  </si>
+  <si>
+    <t>hp_use_best_model</t>
+  </si>
+  <si>
+    <t>mcc_cv</t>
+  </si>
+  <si>
+    <t>model_name</t>
+  </si>
+  <si>
+    <t>submission_number</t>
+  </si>
+  <si>
+    <t>submission_score</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>na_less_50_mixed_upsampling_40_1</t>
+  </si>
+  <si>
+    <t>Logloss</t>
+  </si>
+  <si>
+    <t>catboost</t>
+  </si>
+  <si>
+    <t>TO_FILL</t>
+  </si>
+  <si>
+    <t>2019-12-15T18:25:43.564835</t>
+  </si>
+  <si>
+    <t>2019-12-15T18:26:51.794783</t>
+  </si>
+  <si>
+    <t>na_less_20_median_upsample_00</t>
+  </si>
+  <si>
+    <t>2019-12-15T18:36:45.273840</t>
+  </si>
+  <si>
+    <t>2019-12-15T18:38:21.007376</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>0.003</t>
+  </si>
+  <si>
+    <t>lbm</t>
+  </si>
+  <si>
+    <t>181</t>
+  </si>
+  <si>
+    <t>2019-12-15T18:39:23.745077</t>
+  </si>
+  <si>
+    <t>0.22224</t>
+  </si>
+  <si>
+    <t>0.20365</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,26 +141,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -353,180 +465,226 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>feature_set</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>hp_early_stopping_rounds</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>hp_iterations</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>hp_learning_rate</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>hp_loss_function</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>hp_n_estimators</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>hp_use_best_model</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>mcc_cv</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>model_name</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>submission_number</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>submission_score</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>timestamp</t>
-        </is>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>na_less_50_mixed_upsampling_40_1</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
         <v>100</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>2000</v>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Logloss</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
-        <v>0.2931717839169033</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>catboost</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
+      <c r="H2">
+        <v>0.29317178391690329</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2">
         <v>191</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>TO_FILL</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2019-12-15T18:25:43.564835</t>
-        </is>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>na_less_50_mixed_upsampling_40_1</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>2000</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Logloss</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" t="n">
-        <v>0.2931717839169033</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>catboost</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>192</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>TO_FILL</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>2019-12-15T18:26:51.794783</t>
-        </is>
+      <c r="H3">
+        <v>0.29317178391690329</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3">
+        <v>192</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.20460959617825089</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <v>179</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.20460959617825089</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>180</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>2000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6">
+        <v>0.1562237806432808</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>